<commit_message>
Update Subject data T2DM iHMP (specifying which subjects are not in phyloseq sam_data) 1.1.xlsx
</commit_message>
<xml_diff>
--- a/T2DM iHMP Data/subject data/Subject data T2DM iHMP (specifying which subjects are not in phyloseq sam_data) 1.1.xlsx
+++ b/T2DM iHMP Data/subject data/Subject data T2DM iHMP (specifying which subjects are not in phyloseq sam_data) 1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34420f5773a88cdb/Documents/UM documents/BMS Year 3/Internship ^M Thesis/Sabrina_BMS_Bachelor-Internship/T2DM iHMP Data/subject data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{D172A521-F6EC-4C56-A780-B43F6FA8C789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{637E7E96-6775-4C57-8A05-A4F63ACE73D0}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:1_{D172A521-F6EC-4C56-A780-B43F6FA8C789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DA40D608-EF78-462C-A959-F4E5446656BE}"/>
   <bookViews>
-    <workbookView xWindow="10640" yWindow="0" windowWidth="8600" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,13 +429,13 @@
     <t xml:space="preserve">not in gut 16s data </t>
   </si>
   <si>
-    <t>no of IR and IS subjects with metabolome and gut 16s data that are in the phyloseq sample data</t>
-  </si>
-  <si>
     <t>therefore, 66 - 10 = 56 subjects.</t>
   </si>
   <si>
     <t xml:space="preserve">6 IR and 4 IS subjects with gut 16s and metabolome data not in phyloseq sample data  </t>
+  </si>
+  <si>
+    <t>no of IR and IS subjects with metabolome and gut 16s data that are not in the phyloseq sample data</t>
   </si>
 </sst>
 </file>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1045,7 +1045,7 @@
         <v>131</v>
       </c>
       <c r="M3" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4244,12 +4244,12 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M111" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M112" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>